<commit_message>
Second Fav to Place starts
</commit_message>
<xml_diff>
--- a/Racing_Consolidated.xlsx
+++ b/Racing_Consolidated.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karan\Documents\Code\racing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC4F3003-978B-4CEE-9CEE-71658E60641F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D4A8B7E-BFA0-48AC-BC09-D12EF2E0C16C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet2!$C$9:$G$4233</definedName>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4400" uniqueCount="4153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4439" uniqueCount="4185">
   <si>
     <t>df_bf_raw</t>
   </si>
@@ -12499,6 +12500,102 @@
   </si>
   <si>
     <t>DataFrame = df.runners</t>
+  </si>
+  <si>
+    <t>Track_LIVE</t>
+  </si>
+  <si>
+    <t>MissingOdds</t>
+  </si>
+  <si>
+    <t>Odds</t>
+  </si>
+  <si>
+    <t>Angle Park</t>
+  </si>
+  <si>
+    <t>Casino</t>
+  </si>
+  <si>
+    <t>Christchurch (NZ)</t>
+  </si>
+  <si>
+    <t>Dapto</t>
+  </si>
+  <si>
+    <t>Gawler</t>
+  </si>
+  <si>
+    <t>Gunnedah</t>
+  </si>
+  <si>
+    <t>Hobart</t>
+  </si>
+  <si>
+    <t>Horsham</t>
+  </si>
+  <si>
+    <t>Mandurah</t>
+  </si>
+  <si>
+    <t>Mount Gambier</t>
+  </si>
+  <si>
+    <t>Sandown Park</t>
+  </si>
+  <si>
+    <t>Shepparton</t>
+  </si>
+  <si>
+    <t>Waikato (NZ)</t>
+  </si>
+  <si>
+    <t>Warragul</t>
+  </si>
+  <si>
+    <t>Missing Analysis</t>
+  </si>
+  <si>
+    <t>Date : 02 June 07 07 AM</t>
+  </si>
+  <si>
+    <t>Ballarat</t>
+  </si>
+  <si>
+    <t>Bendigo</t>
+  </si>
+  <si>
+    <t>Cannington</t>
+  </si>
+  <si>
+    <t>Capalaba</t>
+  </si>
+  <si>
+    <t>Darwin</t>
+  </si>
+  <si>
+    <t>Meadows (MEP)</t>
+  </si>
+  <si>
+    <t>Palmerston Nth (NZ)</t>
+  </si>
+  <si>
+    <t>Richmond</t>
+  </si>
+  <si>
+    <t>Rockhampton</t>
+  </si>
+  <si>
+    <t>Taree</t>
+  </si>
+  <si>
+    <t>Traralgon</t>
+  </si>
+  <si>
+    <t>Wentworth Park</t>
+  </si>
+  <si>
+    <t>Date : 01 June 07 37 AM</t>
   </si>
 </sst>
 </file>
@@ -12509,7 +12606,7 @@
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -12528,6 +12625,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -12581,7 +12685,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -12600,6 +12704,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -88865,7 +88970,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D7D1049-098D-4FC3-8E3D-CCFF2376FF25}">
   <dimension ref="C3:H83"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -90212,4 +90317,442 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BB3EAD5-1C46-482A-A27E-51FD9A0BAF4E}">
+  <dimension ref="C3:L21"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.140625" customWidth="1"/>
+    <col min="5" max="5" width="12" customWidth="1"/>
+    <col min="9" max="9" width="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.7109375" customWidth="1"/>
+    <col min="11" max="11" width="13.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>4170</v>
+      </c>
+      <c r="J3" t="s">
+        <v>4170</v>
+      </c>
+    </row>
+    <row r="4" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>4171</v>
+      </c>
+      <c r="J4" t="s">
+        <v>4184</v>
+      </c>
+    </row>
+    <row r="6" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>4153</v>
+      </c>
+      <c r="E6" t="s">
+        <v>4154</v>
+      </c>
+      <c r="F6" t="s">
+        <v>4155</v>
+      </c>
+      <c r="J6" t="s">
+        <v>4153</v>
+      </c>
+      <c r="K6" t="s">
+        <v>4154</v>
+      </c>
+      <c r="L6" t="s">
+        <v>4155</v>
+      </c>
+    </row>
+    <row r="7" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>4075</v>
+      </c>
+      <c r="E7" s="10">
+        <v>94</v>
+      </c>
+      <c r="F7" s="10">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7" s="10" t="s">
+        <v>4075</v>
+      </c>
+      <c r="K7" s="10">
+        <v>109</v>
+      </c>
+      <c r="L7" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>4156</v>
+      </c>
+      <c r="E8" s="10">
+        <v>76</v>
+      </c>
+      <c r="F8" s="10">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8" t="s">
+        <v>4172</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="9" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>4157</v>
+      </c>
+      <c r="E9" s="10">
+        <v>112</v>
+      </c>
+      <c r="F9" s="10">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>2</v>
+      </c>
+      <c r="J9" t="s">
+        <v>4173</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C10">
+        <v>3</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>4158</v>
+      </c>
+      <c r="E10" s="10">
+        <v>120</v>
+      </c>
+      <c r="F10" s="10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>3</v>
+      </c>
+      <c r="J10" s="10" t="s">
+        <v>4174</v>
+      </c>
+      <c r="K10" s="10">
+        <v>104</v>
+      </c>
+      <c r="L10" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C11">
+        <v>4</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>4159</v>
+      </c>
+      <c r="E11" s="10">
+        <v>78</v>
+      </c>
+      <c r="F11" s="10">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>4</v>
+      </c>
+      <c r="J11" s="10" t="s">
+        <v>4175</v>
+      </c>
+      <c r="K11" s="10">
+        <v>81</v>
+      </c>
+      <c r="L11" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C12">
+        <v>5</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>4160</v>
+      </c>
+      <c r="E12" s="10">
+        <v>2</v>
+      </c>
+      <c r="F12" s="10">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>5</v>
+      </c>
+      <c r="J12" s="10" t="s">
+        <v>4176</v>
+      </c>
+      <c r="K12" s="10">
+        <v>60</v>
+      </c>
+      <c r="L12" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C13">
+        <v>6</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>4161</v>
+      </c>
+      <c r="E13" s="10">
+        <v>116</v>
+      </c>
+      <c r="F13" s="10">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>6</v>
+      </c>
+      <c r="J13" s="10" t="s">
+        <v>4160</v>
+      </c>
+      <c r="K13" s="10">
+        <v>101</v>
+      </c>
+      <c r="L13" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C14">
+        <v>7</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>4162</v>
+      </c>
+      <c r="E14" s="10">
+        <v>97</v>
+      </c>
+      <c r="F14" s="10">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>7</v>
+      </c>
+      <c r="J14" t="s">
+        <v>4177</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="15" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C15">
+        <v>8</v>
+      </c>
+      <c r="D15" t="s">
+        <v>4163</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>78</v>
+      </c>
+      <c r="I15">
+        <v>8</v>
+      </c>
+      <c r="J15" s="10" t="s">
+        <v>4178</v>
+      </c>
+      <c r="K15" s="10">
+        <v>70</v>
+      </c>
+      <c r="L15" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C16">
+        <v>9</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>4164</v>
+      </c>
+      <c r="E16" s="10">
+        <v>114</v>
+      </c>
+      <c r="F16" s="10">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>9</v>
+      </c>
+      <c r="J16" s="10" t="s">
+        <v>4179</v>
+      </c>
+      <c r="K16" s="10">
+        <v>109</v>
+      </c>
+      <c r="L16" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C17">
+        <v>10</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>4165</v>
+      </c>
+      <c r="E17" s="10">
+        <v>111</v>
+      </c>
+      <c r="F17" s="10">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>10</v>
+      </c>
+      <c r="J17" s="10" t="s">
+        <v>4180</v>
+      </c>
+      <c r="K17" s="10">
+        <v>78</v>
+      </c>
+      <c r="L17" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C18">
+        <v>11</v>
+      </c>
+      <c r="D18" t="s">
+        <v>4166</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>81</v>
+      </c>
+      <c r="I18">
+        <v>11</v>
+      </c>
+      <c r="J18" s="10" t="s">
+        <v>4181</v>
+      </c>
+      <c r="K18" s="10">
+        <v>105</v>
+      </c>
+      <c r="L18" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C19">
+        <v>12</v>
+      </c>
+      <c r="D19" t="s">
+        <v>4167</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>98</v>
+      </c>
+      <c r="I19">
+        <v>12</v>
+      </c>
+      <c r="J19" t="s">
+        <v>4182</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
+      <c r="L19">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="20" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C20">
+        <v>13</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>4168</v>
+      </c>
+      <c r="E20" s="10">
+        <v>91</v>
+      </c>
+      <c r="F20" s="10">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <v>13</v>
+      </c>
+      <c r="J20" s="10" t="s">
+        <v>4183</v>
+      </c>
+      <c r="K20" s="10">
+        <v>68</v>
+      </c>
+      <c r="L20" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C21">
+        <v>14</v>
+      </c>
+      <c r="D21" t="s">
+        <v>4169</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>93</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update 06 Jun 2022
</commit_message>
<xml_diff>
--- a/Racing_Consolidated.xlsx
+++ b/Racing_Consolidated.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karan\Documents\Code\racing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D4A8B7E-BFA0-48AC-BC09-D12EF2E0C16C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{933D8B61-0C57-4061-A946-E1B537D202C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
+    <sheet name="Live Testing" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet2!$C$9:$G$4233</definedName>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4439" uniqueCount="4185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4470" uniqueCount="4211">
   <si>
     <t>df_bf_raw</t>
   </si>
@@ -12596,6 +12597,84 @@
   </si>
   <si>
     <t>Date : 01 June 07 37 AM</t>
+  </si>
+  <si>
+    <t>strategy</t>
+  </si>
+  <si>
+    <t>races</t>
+  </si>
+  <si>
+    <t>bets</t>
+  </si>
+  <si>
+    <t>profit</t>
+  </si>
+  <si>
+    <t>profitability</t>
+  </si>
+  <si>
+    <t>2_31</t>
+  </si>
+  <si>
+    <t>2_32</t>
+  </si>
+  <si>
+    <t>2_33</t>
+  </si>
+  <si>
+    <t>2_34</t>
+  </si>
+  <si>
+    <t>2_35</t>
+  </si>
+  <si>
+    <t>2_36</t>
+  </si>
+  <si>
+    <t>races_today_live_2022_06_02_07_07.csv</t>
+  </si>
+  <si>
+    <t>dogs_today_live_2022_06_02_07_07.csv</t>
+  </si>
+  <si>
+    <t>RaceId</t>
+  </si>
+  <si>
+    <t>s2_31</t>
+  </si>
+  <si>
+    <t>p2_31</t>
+  </si>
+  <si>
+    <t>s2_32</t>
+  </si>
+  <si>
+    <t>p2_32</t>
+  </si>
+  <si>
+    <t>s2_33</t>
+  </si>
+  <si>
+    <t>p2_33</t>
+  </si>
+  <si>
+    <t>s2_34</t>
+  </si>
+  <si>
+    <t>p2_34</t>
+  </si>
+  <si>
+    <t>s2_35</t>
+  </si>
+  <si>
+    <t>p2_35</t>
+  </si>
+  <si>
+    <t>s2_36</t>
+  </si>
+  <si>
+    <t>p2_36</t>
   </si>
 </sst>
 </file>
@@ -12637,7 +12716,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -12653,6 +12732,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -12685,7 +12770,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -12705,12 +12790,100 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="16">
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -90323,7 +90496,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BB3EAD5-1C46-482A-A27E-51FD9A0BAF4E}">
   <dimension ref="C3:L21"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
@@ -90755,4 +90928,466 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{099A0745-B222-4DC1-A88D-FBF082E1F8D0}">
+  <dimension ref="D6:R22"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" customWidth="1"/>
+    <col min="8" max="8" width="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="6" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>4196</v>
+      </c>
+    </row>
+    <row r="7" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>4197</v>
+      </c>
+    </row>
+    <row r="9" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="E9" s="12" t="s">
+        <v>4185</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>4186</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>4187</v>
+      </c>
+      <c r="H9" s="12" t="s">
+        <v>4188</v>
+      </c>
+      <c r="I9" s="12" t="s">
+        <v>4189</v>
+      </c>
+    </row>
+    <row r="10" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>4190</v>
+      </c>
+      <c r="F10" s="8">
+        <v>47</v>
+      </c>
+      <c r="G10" s="8">
+        <v>48</v>
+      </c>
+      <c r="H10" s="8">
+        <v>1.69999999999999</v>
+      </c>
+      <c r="I10" s="13">
+        <v>3.5000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>4191</v>
+      </c>
+      <c r="F11" s="8">
+        <v>47</v>
+      </c>
+      <c r="G11" s="8">
+        <v>48</v>
+      </c>
+      <c r="H11" s="8">
+        <v>-16.899999999999999</v>
+      </c>
+      <c r="I11" s="13">
+        <v>-0.35199999999999998</v>
+      </c>
+    </row>
+    <row r="12" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D12">
+        <v>2</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>4192</v>
+      </c>
+      <c r="F12" s="8">
+        <v>47</v>
+      </c>
+      <c r="G12" s="8">
+        <v>54</v>
+      </c>
+      <c r="H12" s="8">
+        <v>8.4</v>
+      </c>
+      <c r="I12" s="13">
+        <v>0.156</v>
+      </c>
+    </row>
+    <row r="13" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D13">
+        <v>3</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>4193</v>
+      </c>
+      <c r="F13" s="8">
+        <v>47</v>
+      </c>
+      <c r="G13" s="8">
+        <v>56</v>
+      </c>
+      <c r="H13" s="8">
+        <v>-22</v>
+      </c>
+      <c r="I13" s="13">
+        <v>-0.39300000000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D14">
+        <v>4</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>4194</v>
+      </c>
+      <c r="F14" s="8">
+        <v>47</v>
+      </c>
+      <c r="G14" s="8">
+        <v>52</v>
+      </c>
+      <c r="H14" s="8">
+        <v>-28</v>
+      </c>
+      <c r="I14" s="13">
+        <v>-0.53800000000000003</v>
+      </c>
+    </row>
+    <row r="15" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D15">
+        <v>5</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>4195</v>
+      </c>
+      <c r="F15" s="8">
+        <v>47</v>
+      </c>
+      <c r="G15" s="8">
+        <v>51</v>
+      </c>
+      <c r="H15" s="8">
+        <v>57</v>
+      </c>
+      <c r="I15" s="13">
+        <v>1.1180000000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E18" s="12" t="s">
+        <v>4153</v>
+      </c>
+      <c r="F18" s="12" t="s">
+        <v>4198</v>
+      </c>
+      <c r="G18" s="12" t="s">
+        <v>4199</v>
+      </c>
+      <c r="H18" s="12" t="s">
+        <v>4200</v>
+      </c>
+      <c r="I18" s="12" t="s">
+        <v>4201</v>
+      </c>
+      <c r="J18" s="12" t="s">
+        <v>4202</v>
+      </c>
+      <c r="K18" s="12" t="s">
+        <v>4203</v>
+      </c>
+      <c r="L18" s="12" t="s">
+        <v>4204</v>
+      </c>
+      <c r="M18" s="12" t="s">
+        <v>4205</v>
+      </c>
+      <c r="N18" s="12" t="s">
+        <v>4206</v>
+      </c>
+      <c r="O18" s="12" t="s">
+        <v>4207</v>
+      </c>
+      <c r="P18" s="12" t="s">
+        <v>4208</v>
+      </c>
+      <c r="Q18" s="12" t="s">
+        <v>4209</v>
+      </c>
+      <c r="R18" s="12" t="s">
+        <v>4210</v>
+      </c>
+    </row>
+    <row r="19" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E19" s="11" t="s">
+        <v>4163</v>
+      </c>
+      <c r="F19" s="11">
+        <v>11</v>
+      </c>
+      <c r="G19" s="11">
+        <v>11</v>
+      </c>
+      <c r="H19" s="8">
+        <v>-0.89999999999999902</v>
+      </c>
+      <c r="I19" s="11">
+        <v>11</v>
+      </c>
+      <c r="J19" s="8">
+        <v>9.9999999999999603E-2</v>
+      </c>
+      <c r="K19" s="11">
+        <v>11</v>
+      </c>
+      <c r="L19" s="8">
+        <v>-1.8</v>
+      </c>
+      <c r="M19" s="11">
+        <v>12</v>
+      </c>
+      <c r="N19" s="8">
+        <v>-12</v>
+      </c>
+      <c r="O19" s="11">
+        <v>12</v>
+      </c>
+      <c r="P19" s="8">
+        <v>-4</v>
+      </c>
+      <c r="Q19" s="11">
+        <v>11</v>
+      </c>
+      <c r="R19" s="8">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E20" s="11" t="s">
+        <v>4166</v>
+      </c>
+      <c r="F20" s="11">
+        <v>12</v>
+      </c>
+      <c r="G20" s="11">
+        <v>12</v>
+      </c>
+      <c r="H20" s="8">
+        <v>2.19999999999999</v>
+      </c>
+      <c r="I20" s="11">
+        <v>13</v>
+      </c>
+      <c r="J20" s="8">
+        <v>-4</v>
+      </c>
+      <c r="K20" s="11">
+        <v>14</v>
+      </c>
+      <c r="L20" s="8">
+        <v>6.6</v>
+      </c>
+      <c r="M20" s="11">
+        <v>13</v>
+      </c>
+      <c r="N20" s="8">
+        <v>-5</v>
+      </c>
+      <c r="O20" s="11">
+        <v>12</v>
+      </c>
+      <c r="P20" s="8">
+        <v>-12</v>
+      </c>
+      <c r="Q20" s="11">
+        <v>12</v>
+      </c>
+      <c r="R20" s="8">
+        <v>-12</v>
+      </c>
+    </row>
+    <row r="21" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E21" s="11" t="s">
+        <v>4167</v>
+      </c>
+      <c r="F21" s="11">
+        <v>12</v>
+      </c>
+      <c r="G21" s="11">
+        <v>13</v>
+      </c>
+      <c r="H21" s="8">
+        <v>0.499999999999999</v>
+      </c>
+      <c r="I21" s="11">
+        <v>12</v>
+      </c>
+      <c r="J21" s="8">
+        <v>-12</v>
+      </c>
+      <c r="K21" s="11">
+        <v>14</v>
+      </c>
+      <c r="L21" s="8">
+        <v>7.1</v>
+      </c>
+      <c r="M21" s="11">
+        <v>17</v>
+      </c>
+      <c r="N21" s="8">
+        <v>9</v>
+      </c>
+      <c r="O21" s="11">
+        <v>13</v>
+      </c>
+      <c r="P21" s="8">
+        <v>-13</v>
+      </c>
+      <c r="Q21" s="11">
+        <v>15</v>
+      </c>
+      <c r="R21" s="8">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E22" s="11" t="s">
+        <v>4169</v>
+      </c>
+      <c r="F22" s="11">
+        <v>12</v>
+      </c>
+      <c r="G22" s="11">
+        <v>12</v>
+      </c>
+      <c r="H22" s="8">
+        <v>-9.9999999999999603E-2</v>
+      </c>
+      <c r="I22" s="11">
+        <v>12</v>
+      </c>
+      <c r="J22" s="8">
+        <v>-1</v>
+      </c>
+      <c r="K22" s="11">
+        <v>15</v>
+      </c>
+      <c r="L22" s="8">
+        <v>-3.5</v>
+      </c>
+      <c r="M22" s="11">
+        <v>14</v>
+      </c>
+      <c r="N22" s="8">
+        <v>-14</v>
+      </c>
+      <c r="O22" s="11">
+        <v>15</v>
+      </c>
+      <c r="P22" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q22" s="11">
+        <v>13</v>
+      </c>
+      <c r="R22" s="8">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="E10:I15">
+    <sortCondition ref="E10:E15"/>
+  </sortState>
+  <conditionalFormatting sqref="E10:I15">
+    <cfRule type="cellIs" dxfId="15" priority="14" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H10:I15">
+    <cfRule type="cellIs" dxfId="14" priority="13" operator="greaterThanOrEqual">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H19:H22">
+    <cfRule type="cellIs" dxfId="11" priority="12" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H19:H22">
+    <cfRule type="cellIs" dxfId="10" priority="11" operator="greaterThanOrEqual">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J19:J22">
+    <cfRule type="cellIs" dxfId="9" priority="10" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J19:J22">
+    <cfRule type="cellIs" dxfId="8" priority="9" operator="greaterThanOrEqual">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L19:L22">
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L19:L22">
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="greaterThanOrEqual">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N19:N22">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N19:N22">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="greaterThanOrEqual">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P19:P22">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P19:P22">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="greaterThanOrEqual">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R19:R22">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R19:R22">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThanOrEqual">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>